<commit_message>
Ajout de l'option crazyfli DIY
</commit_message>
<xml_diff>
--- a/comparaison_drone.xlsx
+++ b/comparaison_drone.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a178346e48c8a5e/Stage INRIA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a178346e48c8a5e/Stage INRIA/rapports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_AD4D9D64A577C15A4A541826585B75265ADEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E911E18-5D69-4B37-99FE-921B9616B181}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_AD4D9D64A577C15A4A541826585B75265ADEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E4E46EA-8F04-47AE-8FBC-D5BA26725AF8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>DJI Tello</t>
   </si>
@@ -251,13 +251,28 @@
     <t>DJI Mini 2 / SE</t>
   </si>
   <si>
-    <t>mobile SDK</t>
-  </si>
-  <si>
     <t>https://www.amazon.fr/Ryze-DJI-compatibilit%C3%A9-contr%C3%B4leur-Transmission/dp/B078XV32CJ/ref=sr_1_3?__mk_fr_FR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=16F9VJN29TTJ5&amp;keywords=dji+tello&amp;qid=1643881466&amp;sprefix=dji+tello%2Caps%2C84&amp;sr=8-3</t>
   </si>
   <si>
     <t>350-550€</t>
+  </si>
+  <si>
+    <t>Crazyflie DIY</t>
+  </si>
+  <si>
+    <t>https://www.bitcraze.io/products/old-products/crazyflie-2-0/</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>unlimited</t>
+  </si>
+  <si>
+    <t>mc ESP 32</t>
   </si>
 </sst>
 </file>
@@ -401,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -417,6 +432,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -624,7 +640,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16868775" y="419101"/>
+          <a:off x="17983200" y="419101"/>
           <a:ext cx="2333625" cy="1864594"/>
           <a:chOff x="10001250" y="762001"/>
           <a:chExt cx="2333625" cy="1483594"/>
@@ -743,7 +759,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="19516725" y="523875"/>
+          <a:off x="20631150" y="523875"/>
           <a:ext cx="2990850" cy="1914525"/>
           <a:chOff x="11772900" y="514350"/>
           <a:chExt cx="2990850" cy="1533525"/>
@@ -865,7 +881,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="16811626" y="2466976"/>
+          <a:off x="17926051" y="2466976"/>
           <a:ext cx="2539204" cy="1724025"/>
           <a:chOff x="9277351" y="2381251"/>
           <a:chExt cx="2539204" cy="1390650"/>
@@ -1233,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1246,11 +1262,12 @@
     <col min="3" max="3" width="72.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="46.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="3" customWidth="1"/>
-    <col min="6" max="8" width="11.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="11.5703125" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1266,8 +1283,11 @@
       <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1283,8 +1303,11 @@
       <c r="E2" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1295,13 +1318,13 @@
         <v>550</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="10">
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1317,8 +1340,11 @@
       <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1334,20 +1360,23 @@
       <c r="E5" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="11"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="11"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1363,8 +1392,11 @@
       <c r="E8" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -1380,20 +1412,23 @@
       <c r="E9" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="11"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -1404,13 +1439,16 @@
         <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
         <v>6</v>
@@ -1423,7 +1461,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
       <c r="C14" s="4" t="s">
@@ -1431,7 +1469,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="11"/>
       <c r="C15" s="6" t="s">
@@ -1439,18 +1477,18 @@
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>30</v>
@@ -1458,8 +1496,11 @@
       <c r="D17" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="6" t="s">
@@ -1467,7 +1508,7 @@
       </c>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="6" t="s">
@@ -1475,23 +1516,23 @@
       </c>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>9</v>
       </c>
@@ -1510,13 +1551,14 @@
     <hyperlink ref="E13" r:id="rId10" xr:uid="{06648123-A98B-4506-86A7-27ED158634F2}"/>
     <hyperlink ref="D17" r:id="rId11" xr:uid="{10176AA1-A7C0-49B9-82C4-47ED33305D6D}"/>
     <hyperlink ref="B17" r:id="rId12" xr:uid="{6407FA7A-86F8-4FF5-A94C-D3108756785D}"/>
+    <hyperlink ref="F2" r:id="rId13" xr:uid="{43B70B76-7B5E-4A07-9569-8E907A92FE4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
-  <drawing r:id="rId14"/>
-  <legacyDrawing r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
+  <drawing r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>